<commit_message>
build error and version fixed
</commit_message>
<xml_diff>
--- a/bin/Resoures/InputControl.xlsx
+++ b/bin/Resoures/InputControl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\java workspace\Web_Auto\src\Resoures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DA9111-89F9-4357-9C16-EF17729CC652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9579D72E-CEF5-4D12-9F32-E300A9C1F632}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -486,7 +486,7 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>